<commit_message>
moved spider45 to med4/med4rl/peaks output
</commit_message>
<xml_diff>
--- a/data/ja9-ja16/MED_ETNP_JA14_11.07.17_SPIDER_72/ja14-peptide-spider72.xlsx
+++ b/data/ja9-ja16/MED_ETNP_JA14_11.07.17_SPIDER_72/ja14-peptide-spider72.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/data/ja9-ja16/MED_ETNP_JA14_11.07.17_SPIDER_72/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87FC5DD1-4153-5F46-B414-D70314C0C444}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2CCAB20B-FF40-7A47-8158-2442F1181AE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="4060" windowWidth="27240" windowHeight="16440"/>
+    <workbookView xWindow="2860" yWindow="5020" windowWidth="27240" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="ja14-peptide-spider72" sheetId="1" r:id="rId1"/>
@@ -1694,9 +1694,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">

</xml_diff>